<commit_message>
Unittest for local templates
</commit_message>
<xml_diff>
--- a/src/unittest/excel_file/global_test.xlsx
+++ b/src/unittest/excel_file/global_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="560" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>hostname</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>VLAN</t>
+  </si>
+  <si>
+    <t>VLAN_error</t>
   </si>
 </sst>
 </file>
@@ -678,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" thickTop="1" thickBot="1">
+    <row r="1" spans="1:31" ht="30" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,64 +724,67 @@
         <v>37</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="29" thickTop="1">
+    <row r="2" spans="1:31" ht="29" thickTop="1">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
@@ -810,59 +816,62 @@
       <c r="K2" s="9">
         <v>21</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="9">
+        <v>109</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9">
+      <c r="N2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9">
         <v>101</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="Q2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="9">
         <v>601</v>
       </c>
-      <c r="T2" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="9">
+      <c r="W2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="9">
         <v>901</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="Y2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="9">
+      <c r="AA2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="9">
         <v>21</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="AC2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="AD2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>